<commit_message>
Updated Gains Chart using KS Statistics
</commit_message>
<xml_diff>
--- a/xgb_results.xlsx
+++ b/xgb_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="22">
   <si>
     <t>Trees</t>
   </si>
@@ -34,7 +34,13 @@
     <t>num_vars</t>
   </si>
   <si>
+    <t>Pos Accuracy</t>
+  </si>
+  <si>
     <t>Neg Accuracy</t>
+  </si>
+  <si>
+    <t>F1</t>
   </si>
   <si>
     <t>2</t>
@@ -431,13 +437,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -459,16 +465,22 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D2">
         <v>0.632</v>
@@ -480,18 +492,24 @@
         <v>4</v>
       </c>
       <c r="G2">
-        <v>0.009491733006736069</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="I2">
+        <v>0.019</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D3">
         <v>0.656</v>
@@ -503,18 +521,24 @@
         <v>8</v>
       </c>
       <c r="G3">
-        <v>0.009491733006736069</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="I3">
+        <v>0.019</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D4">
         <v>0.676</v>
@@ -526,18 +550,24 @@
         <v>12</v>
       </c>
       <c r="G4">
-        <v>0.01561543172075934</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>0.999</v>
+      </c>
+      <c r="H4">
+        <v>0.016</v>
+      </c>
+      <c r="I4">
+        <v>0.031</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D5">
         <v>0.6899999999999999</v>
@@ -549,18 +579,24 @@
         <v>20</v>
       </c>
       <c r="G5">
-        <v>0.01561543172075934</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>0.999</v>
+      </c>
+      <c r="H5">
+        <v>0.016</v>
+      </c>
+      <c r="I5">
+        <v>0.031</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D6">
         <v>0.636</v>
@@ -572,18 +608,24 @@
         <v>5</v>
       </c>
       <c r="G6">
-        <v>0.009491733006736069</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="I6">
+        <v>0.019</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D7">
         <v>0.665</v>
@@ -595,18 +637,24 @@
         <v>11</v>
       </c>
       <c r="G7">
-        <v>0.009491733006736069</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="I7">
+        <v>0.019</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D8">
         <v>0.6830000000000001</v>
@@ -618,18 +666,24 @@
         <v>17</v>
       </c>
       <c r="G8">
-        <v>0.01561543172075934</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>0.999</v>
+      </c>
+      <c r="H8">
+        <v>0.016</v>
+      </c>
+      <c r="I8">
+        <v>0.031</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D9">
         <v>0.699</v>
@@ -641,18 +695,24 @@
         <v>26</v>
       </c>
       <c r="G9">
-        <v>0.01500306184935701</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>0.999</v>
+      </c>
+      <c r="H9">
+        <v>0.015</v>
+      </c>
+      <c r="I9">
+        <v>0.029</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D10">
         <v>0.64</v>
@@ -664,18 +724,24 @@
         <v>5</v>
       </c>
       <c r="G10">
-        <v>0.009491733006736069</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="I10">
+        <v>0.019</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D11">
         <v>0.675</v>
@@ -687,18 +753,24 @@
         <v>12</v>
       </c>
       <c r="G11">
-        <v>0.009491733006736069</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="I11">
+        <v>0.019</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D12">
         <v>0.6860000000000001</v>
@@ -710,18 +782,24 @@
         <v>20</v>
       </c>
       <c r="G12">
-        <v>0.01469687691365585</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>0.999</v>
+      </c>
+      <c r="H12">
+        <v>0.015</v>
+      </c>
+      <c r="I12">
+        <v>0.029</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D13">
         <v>0.701</v>
@@ -733,18 +811,24 @@
         <v>30</v>
       </c>
       <c r="G13">
-        <v>0.01285976729944887</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>0.999</v>
+      </c>
+      <c r="H13">
+        <v>0.013</v>
+      </c>
+      <c r="I13">
+        <v>0.025</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D14">
         <v>0.65</v>
@@ -756,18 +840,24 @@
         <v>5</v>
       </c>
       <c r="G14">
-        <v>0.009491733006736069</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="I14">
+        <v>0.019</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
         <v>10</v>
       </c>
-      <c r="B15" t="s">
-        <v>8</v>
-      </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D15">
         <v>0.675</v>
@@ -779,18 +869,24 @@
         <v>13</v>
       </c>
       <c r="G15">
-        <v>0.009491733006736069</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="I15">
+        <v>0.019</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D16">
         <v>0.6909999999999999</v>
@@ -802,18 +898,24 @@
         <v>24</v>
       </c>
       <c r="G16">
-        <v>0.01132884262094305</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>0.011</v>
+      </c>
+      <c r="I16">
+        <v>0.022</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D17">
         <v>0.706</v>
@@ -825,18 +927,24 @@
         <v>39</v>
       </c>
       <c r="G17">
-        <v>0.01163502755664421</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>0.012</v>
+      </c>
+      <c r="I17">
+        <v>0.023</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D18">
         <v>0.663</v>
@@ -848,18 +956,24 @@
         <v>5</v>
       </c>
       <c r="G18">
-        <v>0.009491733006736069</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="I18">
+        <v>0.019</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D19">
         <v>0.679</v>
@@ -871,18 +985,24 @@
         <v>14</v>
       </c>
       <c r="G19">
-        <v>0.009491733006736069</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="I19">
+        <v>0.019</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" t="s">
         <v>11</v>
       </c>
-      <c r="B20" t="s">
-        <v>9</v>
-      </c>
       <c r="C20" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D20">
         <v>0.6919999999999999</v>
@@ -894,18 +1014,24 @@
         <v>26</v>
       </c>
       <c r="G20">
-        <v>0.01316595223515003</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>0.999</v>
+      </c>
+      <c r="H20">
+        <v>0.013</v>
+      </c>
+      <c r="I20">
+        <v>0.026</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D21">
         <v>0.707</v>
@@ -917,18 +1043,24 @@
         <v>42</v>
       </c>
       <c r="G21">
-        <v>0.01194121249234538</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>0.999</v>
+      </c>
+      <c r="H21">
+        <v>0.012</v>
+      </c>
+      <c r="I21">
+        <v>0.024</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D22">
         <v>0.671</v>
@@ -940,18 +1072,24 @@
         <v>7</v>
       </c>
       <c r="G22">
-        <v>0.009491733006736069</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="I22">
+        <v>0.019</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D23">
         <v>0.6860000000000001</v>
@@ -963,18 +1101,24 @@
         <v>15</v>
       </c>
       <c r="G23">
-        <v>0.009491733006736069</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="I23">
+        <v>0.019</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D24">
         <v>0.697</v>
@@ -986,18 +1130,24 @@
         <v>28</v>
       </c>
       <c r="G24">
-        <v>0.01132884262094305</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>0.011</v>
+      </c>
+      <c r="I24">
+        <v>0.022</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" t="s">
         <v>12</v>
       </c>
-      <c r="B25" t="s">
-        <v>10</v>
-      </c>
       <c r="C25" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D25">
         <v>0.712</v>
@@ -1009,18 +1159,24 @@
         <v>45</v>
       </c>
       <c r="G25">
-        <v>0.01102265768524189</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>0.011</v>
+      </c>
+      <c r="I25">
+        <v>0.022</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D26">
         <v>0.67</v>
@@ -1032,18 +1188,24 @@
         <v>7</v>
       </c>
       <c r="G26">
-        <v>0.009491733006736069</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="I26">
+        <v>0.019</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B27" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D27">
         <v>0.6850000000000001</v>
@@ -1055,18 +1217,24 @@
         <v>15</v>
       </c>
       <c r="G27">
-        <v>0.009491733006736069</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="I27">
+        <v>0.019</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B28" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C28" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D28">
         <v>0.7</v>
@@ -1078,18 +1246,24 @@
         <v>29</v>
       </c>
       <c r="G28">
-        <v>0.01102265768524189</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>0.011</v>
+      </c>
+      <c r="I28">
+        <v>0.022</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B29" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C29" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D29">
         <v>0.712</v>
@@ -1101,18 +1275,24 @@
         <v>46</v>
       </c>
       <c r="G29">
-        <v>0.01163502755664421</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>0.012</v>
+      </c>
+      <c r="I29">
+        <v>0.023</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C30" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D30">
         <v>0.673</v>
@@ -1124,18 +1304,24 @@
         <v>7</v>
       </c>
       <c r="G30">
-        <v>0.009491733006736069</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="I30">
+        <v>0.019</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D31">
         <v>0.6870000000000001</v>
@@ -1147,18 +1333,24 @@
         <v>16</v>
       </c>
       <c r="G31">
-        <v>0.009491733006736069</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="I31">
+        <v>0.019</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C32" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D32">
         <v>0.702</v>
@@ -1170,18 +1362,24 @@
         <v>31</v>
       </c>
       <c r="G32">
-        <v>0.01071647274954072</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>0.011</v>
+      </c>
+      <c r="I32">
+        <v>0.021</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C33" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D33">
         <v>0.714</v>
@@ -1193,18 +1391,24 @@
         <v>49</v>
       </c>
       <c r="G33">
-        <v>0.01224739742804654</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+        <v>0.999</v>
+      </c>
+      <c r="H33">
+        <v>0.012</v>
+      </c>
+      <c r="I33">
+        <v>0.024</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B34" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C34" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D34">
         <v>0.679</v>
@@ -1216,18 +1420,24 @@
         <v>8</v>
       </c>
       <c r="G34">
-        <v>0.009491733006736069</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H34">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="I34">
+        <v>0.019</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B35" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C35" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D35">
         <v>0.6919999999999999</v>
@@ -1239,18 +1449,24 @@
         <v>17</v>
       </c>
       <c r="G35">
-        <v>0.009491733006736069</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="I35">
+        <v>0.019</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B36" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C36" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D36">
         <v>0.707</v>
@@ -1262,18 +1478,24 @@
         <v>32</v>
       </c>
       <c r="G36">
-        <v>0.01041028781383956</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H36">
+        <v>0.01</v>
+      </c>
+      <c r="I36">
+        <v>0.021</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B37" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C37" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D37">
         <v>0.717</v>
@@ -1285,18 +1507,24 @@
         <v>55</v>
       </c>
       <c r="G37">
-        <v>0.01194121249234538</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
+        <v>0.999</v>
+      </c>
+      <c r="H37">
+        <v>0.012</v>
+      </c>
+      <c r="I37">
+        <v>0.024</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B38" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C38" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D38">
         <v>0.68</v>
@@ -1308,18 +1536,24 @@
         <v>9</v>
       </c>
       <c r="G38">
-        <v>0.009491733006736069</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H38">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="I38">
+        <v>0.019</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B39" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C39" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D39">
         <v>0.694</v>
@@ -1331,18 +1565,24 @@
         <v>18</v>
       </c>
       <c r="G39">
-        <v>0.009491733006736069</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="I39">
+        <v>0.019</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B40" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C40" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D40">
         <v>0.709</v>
@@ -1354,18 +1594,24 @@
         <v>36</v>
       </c>
       <c r="G40">
-        <v>0.01041028781383956</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H40">
+        <v>0.01</v>
+      </c>
+      <c r="I40">
+        <v>0.021</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B41" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C41" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D41">
         <v>0.721</v>
@@ -1377,18 +1623,24 @@
         <v>65</v>
       </c>
       <c r="G41">
-        <v>0.01224739742804654</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H41">
+        <v>0.012</v>
+      </c>
+      <c r="I41">
+        <v>0.024</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B42" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C42" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D42">
         <v>0.6850000000000001</v>
@@ -1400,18 +1652,24 @@
         <v>10</v>
       </c>
       <c r="G42">
-        <v>0.009185548071034905</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H42">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="I42">
+        <v>0.018</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B43" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C43" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D43">
         <v>0.699</v>
@@ -1423,18 +1681,24 @@
         <v>20</v>
       </c>
       <c r="G43">
-        <v>0.009491733006736069</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H43">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="I43">
+        <v>0.019</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B44" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C44" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D44">
         <v>0.713</v>
@@ -1446,18 +1710,24 @@
         <v>38</v>
       </c>
       <c r="G44">
-        <v>0.01102265768524189</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H44">
+        <v>0.011</v>
+      </c>
+      <c r="I44">
+        <v>0.022</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B45" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C45" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D45">
         <v>0.726</v>
@@ -1469,18 +1739,24 @@
         <v>72</v>
       </c>
       <c r="G45">
-        <v>0.01194121249234538</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H45">
+        <v>0.012</v>
+      </c>
+      <c r="I45">
+        <v>0.024</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B46" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C46" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D46">
         <v>0.6919999999999999</v>
@@ -1492,18 +1768,24 @@
         <v>13</v>
       </c>
       <c r="G46">
-        <v>0.008879363135333742</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H46">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="I46">
+        <v>0.018</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B47" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C47" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D47">
         <v>0.707</v>
@@ -1515,18 +1797,24 @@
         <v>23</v>
       </c>
       <c r="G47">
-        <v>0.009491733006736069</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H47">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="I47">
+        <v>0.019</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B48" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C48" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D48">
         <v>0.718</v>
@@ -1538,18 +1826,24 @@
         <v>45</v>
       </c>
       <c r="G48">
-        <v>0.01102265768524189</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H48">
+        <v>0.011</v>
+      </c>
+      <c r="I48">
+        <v>0.022</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B49" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C49" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D49">
         <v>0.734</v>
@@ -1561,7 +1855,13 @@
         <v>78</v>
       </c>
       <c r="G49">
-        <v>0.01224739742804654</v>
+        <v>0.999</v>
+      </c>
+      <c r="H49">
+        <v>0.012</v>
+      </c>
+      <c r="I49">
+        <v>0.024</v>
       </c>
     </row>
   </sheetData>

</xml_diff>